<commit_message>
Dec 20 hacking update
</commit_message>
<xml_diff>
--- a/project/excel/hdmf_term_lists.xlsx
+++ b/project/excel/hdmf_term_lists.xlsx
@@ -4,15 +4,21 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="11" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Subject" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="SubjectCollection" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="NamedThing1" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Subject1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="SubjectCollection1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ElectricalArray" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Electrode" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ElectrodeSeries" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="OneDimensionalSeries" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TimestampSeries" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TwoDimensionalArray" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="ElectricalArray1" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Electrode1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ElectrodeSeries1" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="OneDimensionalSeries1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="TimestampSeries1" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="TwoDimensionalArray1" sheetId="12" state="visible" r:id="rId12"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,17 +435,125 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>ElectricalArray_axis0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ElectricalArray_axis1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ElectricalArray_values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TimestampSeries_data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>TimestampSeries_values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>twoDimensionalArray__axis0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>twoDimensionalArray__axis1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>twoDimensionalArray__values</t>
         </is>
       </c>
     </row>
@@ -454,60 +568,22 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Subject_primary_email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation sqref="G2:G1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-    <dataValidation sqref="G2:G1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>electrode__impedance</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -518,6 +594,186 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ElectrodeSeries_values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TimestampSeries_data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>TimestampSeries_values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>twoDimensionalArray__axis0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>twoDimensionalArray__axis1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>twoDimensionalArray__values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ElectricalArray_axis0</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>ElectricalArray_axis1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ElectricalArray_values</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -529,125 +785,43 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>subjectCollection__entries</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Subject_primary_email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>birth_date</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>age_in_years</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>vital_status</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>subjectCollection__entries</t>
+          <t>electrode__impedance</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>oneDimensionalSeries__data_type</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ElectrodeSeries_values</t>
         </is>
       </c>
     </row>

</xml_diff>